<commit_message>
Reorganize plots and regenarate tables
</commit_message>
<xml_diff>
--- a/Results/One_Mutation_File.xlsx
+++ b/Results/One_Mutation_File.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor</t>
   </si>
@@ -64,52 +64,136 @@
     <t xml:space="preserve">Norm_Mean_Size_Difference</t>
   </si>
   <si>
+    <t xml:space="preserve">0.54985754985755</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.666666666666667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.743589743589744</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.766381766381766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.773504273504273</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.857549857549857</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.908831908831909</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.931623931623932</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.977207977207977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.994301994301994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Untreated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
     <t xml:space="preserve">GLI_Inhibitor + NFKB_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.407407407407407</t>
   </si>
   <si>
     <t xml:space="preserve">AKT_Inhibitor + STAT3_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.41025641025641</t>
+  </si>
+  <si>
     <t xml:space="preserve">AKT_Inhibitor + NFKB_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.421652421652422</t>
   </si>
   <si>
     <t xml:space="preserve">NFKB_Inhibitor + CREB_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.43019943019943</t>
+  </si>
+  <si>
     <t xml:space="preserve">NFKB_Inhibitor + STAT3_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.435897435897436</t>
   </si>
   <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + NFKB_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.458689458689459</t>
+  </si>
+  <si>
     <t xml:space="preserve">NFKB_Inhibitor + PI3K_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.46011396011396</t>
   </si>
   <si>
     <t xml:space="preserve">CREB_Inhibitor + STAT3_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.50997150997151</t>
+  </si>
+  <si>
     <t xml:space="preserve">STAT3_Inhibitor + PI3K_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.517094017094017</t>
   </si>
   <si>
     <t xml:space="preserve">GLI_Inhibitor + AKT_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.524216524216524</t>
+  </si>
+  <si>
     <t xml:space="preserve">GLI_Inhibitor + AKT_Inhibitor + STAT3_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.267806267806268</t>
   </si>
   <si>
     <t xml:space="preserve">GLI_Inhibitor + AKT_Inhibitor + NFKB_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.279202279202279</t>
+  </si>
+  <si>
     <t xml:space="preserve">GLI_Inhibitor + NFKB_Inhibitor + CREB_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.287749287749288</t>
   </si>
   <si>
     <t xml:space="preserve">GLI_Inhibitor + NFKB_Inhibitor + STAT3_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.293447293447293</t>
+  </si>
+  <si>
     <t xml:space="preserve">AKT_Inhibitor + NFKB_Inhibitor + STAT3_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.307692307692308</t>
+  </si>
+  <si>
     <t xml:space="preserve">NFKB_Inhibitor + CREB_Inhibitor + STAT3_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.316239316239316</t>
   </si>
   <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + GLI_Inhibitor + NFKB_Inhibitor</t>
@@ -118,70 +202,139 @@
     <t xml:space="preserve">GLI_Inhibitor + NFKB_Inhibitor + PI3K_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.317663817663818</t>
+  </si>
+  <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + AKT_Inhibitor + STAT3_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.319088319088319</t>
   </si>
   <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + AKT_Inhibitor + NFKB_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.33048433048433</t>
+  </si>
+  <si>
     <t xml:space="preserve">GLI_Inhibitor + AKT_Inhibitor + NFKB_Inhibitor + STAT3_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.165242165242165</t>
   </si>
   <si>
     <t xml:space="preserve">GLI_Inhibitor + NFKB_Inhibitor + CREB_Inhibitor + STAT3_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.173789173789174</t>
+  </si>
+  <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + GLI_Inhibitor + AKT_Inhibitor + STAT3_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.176638176638177</t>
   </si>
   <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + GLI_Inhibitor + AKT_Inhibitor + NFKB_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.188034188034188</t>
+  </si>
+  <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + GLI_Inhibitor + NFKB_Inhibitor + CREB_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.196581196581197</t>
   </si>
   <si>
     <t xml:space="preserve">GLI_Inhibitor + Notch_complex_Inhibitor + AKT_Inhibitor + STAT3_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.199430199430199</t>
+  </si>
+  <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + GLI_Inhibitor + NFKB_Inhibitor + STAT3_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.202279202279202</t>
   </si>
   <si>
     <t xml:space="preserve">GLI_Inhibitor + NFKB_Inhibitor + STAT3_Inhibitor + PI3K_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.203703703703704</t>
+  </si>
+  <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + AKT_Inhibitor + NFKB_Inhibitor + STAT3_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.216524216524217</t>
   </si>
   <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + NFKB_Inhibitor + CREB_Inhibitor + STAT3_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.225071225071225</t>
+  </si>
+  <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + GLI_Inhibitor + AKT_Inhibitor + NFKB_Inhibitor + STAT3_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0740740740740741</t>
   </si>
   <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + GLI_Inhibitor + NFKB_Inhibitor + CREB_Inhibitor + STAT3_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.0826210826210826</t>
+  </si>
+  <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + GLI_Inhibitor + Notch_complex_Inhibitor + AKT_Inhibitor + STAT3_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.108262108262108</t>
   </si>
   <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + GLI_Inhibitor + NFKB_Inhibitor + STAT3_Inhibitor + PI3K_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.112535612535613</t>
+  </si>
+  <si>
     <t xml:space="preserve">GLI_Inhibitor + AKT_Inhibitor + NFKB_Inhibitor + STAT3_Inhibitor + Hippo_complex_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.142450142450142</t>
   </si>
   <si>
     <t xml:space="preserve">GLI_Inhibitor + Notch_complex_Inhibitor + AKT_Inhibitor + NFKB_Inhibitor + STAT3_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.148148148148148</t>
+  </si>
+  <si>
     <t xml:space="preserve">GLI_Inhibitor + NFKB_Inhibitor + CREB_Inhibitor + STAT3_Inhibitor + Hippo_complex_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.150997150997151</t>
   </si>
   <si>
     <t xml:space="preserve">Beta_Catenin_complex_Inhibitor + GLI_Inhibitor + AKT_Inhibitor + STAT3_Inhibitor + Hippo_complex_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.153846153846154</t>
+  </si>
+  <si>
     <t xml:space="preserve">GLI_Inhibitor + Notch_complex_Inhibitor + NFKB_Inhibitor + CREB_Inhibitor + STAT3_Inhibitor</t>
   </si>
   <si>
+    <t xml:space="preserve">0.156695156695157</t>
+  </si>
+  <si>
     <t xml:space="preserve">GLI_Inhibitor + AKT_Inhibitor + NFKB_Inhibitor + CREB_Inhibitor + STAT3_Inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.15954415954416</t>
   </si>
 </sst>
 </file>
@@ -42564,80 +42717,88 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.54985754985755</v>
+      <c r="B2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="n">
-        <v>0.666666666666667</v>
+      <c r="B3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="n">
-        <v>0.743589743589744</v>
+      <c r="B4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="n">
-        <v>0.766381766381766</v>
+      <c r="B5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="n">
-        <v>0.773504273504273</v>
+      <c r="B6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" t="n">
-        <v>0.857549857549857</v>
+      <c r="B7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" t="n">
-        <v>0.908831908831909</v>
+      <c r="B8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" t="n">
-        <v>0.931623931623932</v>
+      <c r="B9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="n">
-        <v>0.977207977207977</v>
+      <c r="B10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" t="n">
-        <v>0.994301994301994</v>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -42664,82 +42825,90 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.407407407407407</v>
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.41025641025641</v>
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.421652421652422</v>
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.43019943019943</v>
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.435897435897436</v>
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.458689458689459</v>
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.46011396011396</v>
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.50997150997151</v>
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.517094017094017</v>
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.524216524216524</v>
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -42766,82 +42935,90 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.267806267806268</v>
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.279202279202279</v>
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.287749287749288</v>
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.293447293447293</v>
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.307692307692308</v>
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.316239316239316</v>
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.316239316239316</v>
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.317663817663818</v>
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.319088319088319</v>
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.33048433048433</v>
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -42868,82 +43045,90 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.165242165242165</v>
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.173789173789174</v>
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.176638176638177</v>
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.188034188034188</v>
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.196581196581197</v>
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.199430199430199</v>
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.202279202279202</v>
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.203703703703704</v>
+        <v>80</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.216524216524217</v>
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.225071225071225</v>
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -42970,82 +43155,90 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.0740740740740741</v>
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.0826210826210826</v>
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.108262108262108</v>
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.112535612535613</v>
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.142450142450142</v>
+        <v>94</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.148148148148148</v>
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.150997150997151</v>
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.153846153846154</v>
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.156695156695157</v>
+        <v>102</v>
+      </c>
+      <c r="B10" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.15954415954416</v>
+        <v>104</v>
+      </c>
+      <c r="B11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>